<commit_message>
feat: add excel edit
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t xml:space="preserve">Ip</t>
   </si>
@@ -97,6 +97,21 @@
     <t xml:space="preserve">Comentario</t>
   </si>
   <si>
+    <t xml:space="preserve">Garantías Propuestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo Garantía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo bien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor Comercial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripcion</t>
+  </si>
+  <si>
     <t xml:space="preserve">10.16.5.64</t>
   </si>
   <si>
@@ -176,6 +191,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERRENO</t>
   </si>
 </sst>
 </file>
@@ -260,13 +287,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -296,8 +327,8 @@
   </sheetPr>
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -307,7 +338,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -388,126 +419,151 @@
       </c>
       <c r="AA1" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="N2" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="T2" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="2"/>
-      <c r="AW2" s="2"/>
-      <c r="AX2" s="2"/>
-      <c r="AY2" s="2"/>
-      <c r="AZ2" s="2"/>
-      <c r="BA2" s="2"/>
-      <c r="BB2" s="2"/>
-      <c r="BC2" s="2"/>
-      <c r="BD2" s="2"/>
-      <c r="BE2" s="2"/>
-      <c r="BF2" s="2"/>
-      <c r="BG2" s="2"/>
-      <c r="BH2" s="2"/>
-      <c r="BI2" s="2"/>
-      <c r="BJ2" s="2"/>
-      <c r="BK2" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3"/>
+      <c r="AW2" s="3"/>
+      <c r="AX2" s="3"/>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="3"/>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="3"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
+      <c r="BI2" s="3"/>
+      <c r="BJ2" s="3"/>
+      <c r="BK2" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: add transaction 00-0267
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t xml:space="preserve">Ip</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t xml:space="preserve">TERRENO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-0267</t>
   </si>
 </sst>
 </file>
@@ -327,8 +330,8 @@
   </sheetPr>
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,6 +438,9 @@
       <c r="AF1" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="AG1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -533,7 +539,9 @@
       <c r="AF2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AG2" s="3"/>
+      <c r="AG2" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>

</xml_diff>

<commit_message>
feat: add transaction 063040
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t xml:space="preserve">Ip</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t xml:space="preserve">06-3071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-3040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROBADO</t>
   </si>
 </sst>
 </file>
@@ -333,8 +339,8 @@
   </sheetPr>
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH2" activeCellId="0" sqref="AH2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,6 +453,12 @@
       <c r="AH1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="AI1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -551,8 +563,12 @@
       <c r="AH2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
+      <c r="AI2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>

</xml_diff>

<commit_message>
feat: add tr063080 complete
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
   <si>
     <t xml:space="preserve">Ip</t>
   </si>
@@ -130,7 +130,25 @@
     <t xml:space="preserve">Conclusión CP</t>
   </si>
   <si>
-    <t xml:space="preserve">10.16.5.64</t>
+    <t xml:space="preserve">Cumple Política De Garantías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobertura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumple Requisitos Documentales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacidad De Pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limite De Endeudamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviar Aprobación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.16.5.64</t>
   </si>
   <si>
     <t xml:space="preserve">UE0100061Y</t>
@@ -367,7 +385,7 @@
   <dimension ref="A1:BK9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -507,140 +525,170 @@
       <c r="AP1" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="AQ1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="AC2" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
       <c r="AY2" s="3"/>

</xml_diff>

<commit_message>
feat: add block code
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Enviar Aprobación</t>
   </si>
   <si>
-    <t xml:space="preserve">10.16.5.64</t>
+    <t xml:space="preserve">10.1.115.64</t>
   </si>
   <si>
     <t xml:space="preserve">UE0100061Y</t>
@@ -385,7 +385,7 @@
   <dimension ref="A1:BK9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: add incognito browser
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -393,8 +393,8 @@
   </sheetPr>
   <dimension ref="A1:BK9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW1" activeCellId="0" sqref="AW1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: add tr062033 tr062001
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t xml:space="preserve">Ip</t>
   </si>
@@ -151,6 +151,15 @@
     <t xml:space="preserve">Tipo Transaccion</t>
   </si>
   <si>
+    <t xml:space="preserve">Transacción 06-2033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comentario de 06-2033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transacción 06-2001</t>
+  </si>
+  <si>
     <t xml:space="preserve">10.16.5.64</t>
   </si>
   <si>
@@ -269,6 +278,12 @@
   </si>
   <si>
     <t xml:space="preserve">3080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-2033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-2001</t>
   </si>
 </sst>
 </file>
@@ -558,161 +573,176 @@
       <c r="AX1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="AY1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA1" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="AC2" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AP2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AQ2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AW2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY2" s="3"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
+      <c r="BA2" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="BB2" s="3"/>
       <c r="BC2" s="3"/>
       <c r="BD2" s="3"/>

</xml_diff>

<commit_message>
fix: resolve error 06-2001
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -160,7 +160,7 @@
     <t xml:space="preserve">Transacción 06-2001</t>
   </si>
   <si>
-    <t xml:space="preserve">10.16.5.64</t>
+    <t xml:space="preserve">10.15.6.64</t>
   </si>
   <si>
     <t xml:space="preserve">UE0100061Y</t>
@@ -422,7 +422,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -589,7 +589,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="4" t="s">

</xml_diff>

<commit_message>
feat: add transaction 06-2001
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/testRead02.xlsx
+++ b/src/test/assets/exceldocuments/testRead02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="90">
   <si>
     <t xml:space="preserve">Ip</t>
   </si>
@@ -160,7 +160,10 @@
     <t xml:space="preserve">Transacción 06-2001</t>
   </si>
   <si>
-    <t xml:space="preserve">10.15.6.64</t>
+    <t xml:space="preserve">Decisión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.16.5.64</t>
   </si>
   <si>
     <t xml:space="preserve">UE0100061Y</t>
@@ -284,6 +287,9 @@
   </si>
   <si>
     <t xml:space="preserve">06-2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROBAR</t>
   </si>
 </sst>
 </file>
@@ -416,13 +422,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BD2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -587,169 +593,181 @@
       <c r="BB1" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="BC1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="AC2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AX2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AL2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="BB2" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="BC2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD2" s="1" t="n">
+        <v>2001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>